<commit_message>
Envío de correos desde energias.renovables.es@dekra.com
</commit_message>
<xml_diff>
--- a/informe_mtto_LIDARS.xlsx
+++ b/informe_mtto_LIDARS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\EOLICA\MAT REF\BASE DE DATOS ESTACIONES\control_LiDARS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A510633\Desktop\Javi\control_LiDARS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79487AAA-CFBD-4C0A-9DFD-2D49C661CBA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAF635B-2AFB-4C93-A945-A8BF97DBA4B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -918,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
@@ -1052,7 +1052,7 @@
         <v>33</v>
       </c>
       <c r="R2" s="63">
-        <v>45930.493055555555</v>
+        <v>45930.531944444447</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>36</v>

</xml_diff>